<commit_message>
Add 2022 mortality data
</commit_message>
<xml_diff>
--- a/Figures_Tables/Supp_Table_1.xlsx
+++ b/Figures_Tables/Supp_Table_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">ICD10_groups</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022</t>
   </si>
   <si>
     <t xml:space="preserve">Chronic lower
@@ -494,10 +497,13 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="n">
         <v>23</v>
@@ -549,11 +555,14 @@
       </c>
       <c r="R2" t="n">
         <v>14</v>
+      </c>
+      <c r="S2" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>35</v>
@@ -605,11 +614,14 @@
       </c>
       <c r="R3" t="n">
         <v>25</v>
+      </c>
+      <c r="S3" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
         <v>362</v>
@@ -661,11 +673,14 @@
       </c>
       <c r="R4" t="n">
         <v>108</v>
+      </c>
+      <c r="S4" t="n">
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
         <v>76</v>
@@ -717,11 +732,14 @@
       </c>
       <c r="R5" t="n">
         <v>18</v>
+      </c>
+      <c r="S5" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
         <v>35</v>
@@ -773,11 +791,14 @@
       </c>
       <c r="R6" t="n">
         <v>10</v>
+      </c>
+      <c r="S6" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>332</v>
@@ -829,11 +850,14 @@
       </c>
       <c r="R7" t="n">
         <v>89</v>
+      </c>
+      <c r="S7" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n">
         <v>295</v>
@@ -885,11 +909,14 @@
       </c>
       <c r="R8" t="n">
         <v>65</v>
+      </c>
+      <c r="S8" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="n">
         <v>8</v>
@@ -941,11 +968,14 @@
       </c>
       <c r="R9" t="n">
         <v>9</v>
+      </c>
+      <c r="S9" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -997,6 +1027,9 @@
       </c>
       <c r="R10" t="n">
         <v>118</v>
+      </c>
+      <c r="S10" t="n">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>